<commit_message>
fixed bag with y cpunt
</commit_message>
<xml_diff>
--- a/GenerateApp/tables_long_horiz/Data/10/source.xlsx
+++ b/GenerateApp/tables_long_horiz/Data/10/source.xlsx
@@ -69,215 +69,101 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="C0C0C0"/>
+              <a:srgbClr val="800000"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$32</c:f>
+              <c:f>Sheet1!$A$1:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1978</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1979</c:v>
+                  <c:v>2001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1980</c:v>
+                  <c:v>2002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1981</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1982</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1983</c:v>
+                  <c:v>2005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1984</c:v>
+                  <c:v>2006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1985</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1986</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1987</c:v>
+                  <c:v>2009</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1988</c:v>
+                  <c:v>2010</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1989</c:v>
+                  <c:v>2011</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1990</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1991</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1992</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1993</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1994</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1995</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1996</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2009</c:v>
+                  <c:v>2012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$32</c:f>
+              <c:f>Sheet1!$B$1:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>444</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>896</c:v>
+                  <c:v>479</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>431</c:v>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>741</c:v>
+                  <c:v>517</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>580</c:v>
+                  <c:v>598</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>635</c:v>
+                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>766</c:v>
+                  <c:v>581</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>402</c:v>
+                  <c:v>469</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>725</c:v>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>711</c:v>
+                  <c:v>506</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>514</c:v>
+                  <c:v>597</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>742</c:v>
+                  <c:v>441</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>408</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>783</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>453</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>532</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>702</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>702</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>528</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>717</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>444</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>493</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>459</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>659</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>878</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>923</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>844</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>468</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>673</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>510</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>834</c:v>
+                  <c:v>499</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -299,7 +185,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="975" baseline="0"/>
+              <a:defRPr sz="650" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -352,10 +240,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -662,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -670,258 +558,106 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">
-        <v>1978</v>
+        <v>2000</v>
       </c>
       <c r="B1">
-        <v>444</v>
+        <v>450</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>1979</v>
+        <v>2001</v>
       </c>
       <c r="B2">
-        <v>896</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>1980</v>
+        <v>2002</v>
       </c>
       <c r="B3">
-        <v>431</v>
+        <v>466</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>1981</v>
+        <v>2003</v>
       </c>
       <c r="B4">
-        <v>741</v>
+        <v>517</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>1982</v>
+        <v>2004</v>
       </c>
       <c r="B5">
-        <v>580</v>
+        <v>598</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>1983</v>
+        <v>2005</v>
       </c>
       <c r="B6">
-        <v>635</v>
+        <v>482</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>1984</v>
+        <v>2006</v>
       </c>
       <c r="B7">
-        <v>766</v>
+        <v>581</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>1985</v>
+        <v>2007</v>
       </c>
       <c r="B8">
-        <v>402</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>1986</v>
+        <v>2008</v>
       </c>
       <c r="B9">
-        <v>725</v>
+        <v>466</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>1987</v>
+        <v>2009</v>
       </c>
       <c r="B10">
-        <v>711</v>
+        <v>506</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>1988</v>
+        <v>2010</v>
       </c>
       <c r="B11">
-        <v>514</v>
+        <v>597</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>1989</v>
+        <v>2011</v>
       </c>
       <c r="B12">
-        <v>742</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>1990</v>
+        <v>2012</v>
       </c>
       <c r="B13">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>1991</v>
-      </c>
-      <c r="B14">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>1992</v>
-      </c>
-      <c r="B15">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
-        <v>1993</v>
-      </c>
-      <c r="B16">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>1994</v>
-      </c>
-      <c r="B17">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>1995</v>
-      </c>
-      <c r="B18">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
-        <v>1996</v>
-      </c>
-      <c r="B19">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
-        <v>1997</v>
-      </c>
-      <c r="B20">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
-        <v>1998</v>
-      </c>
-      <c r="B21">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
-        <v>1999</v>
-      </c>
-      <c r="B22">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
-        <v>2000</v>
-      </c>
-      <c r="B23">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
-        <v>2001</v>
-      </c>
-      <c r="B24">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25">
-        <v>2002</v>
-      </c>
-      <c r="B25">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
-        <v>2003</v>
-      </c>
-      <c r="B26">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27">
-        <v>2004</v>
-      </c>
-      <c r="B27">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28">
-        <v>2005</v>
-      </c>
-      <c r="B28">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29">
-        <v>2006</v>
-      </c>
-      <c r="B29">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30">
-        <v>2007</v>
-      </c>
-      <c r="B30">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31">
-        <v>2008</v>
-      </c>
-      <c r="B31">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32">
-        <v>2009</v>
-      </c>
-      <c r="B32">
-        <v>834</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>